<commit_message>
Added more PDOs to the logger, added files
</commit_message>
<xml_diff>
--- a/Datalogger V2/Commands.xlsx
+++ b/Datalogger V2/Commands.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>sudo apt-get update; sudo apt-get upgrade</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>setup RPI-Wireless_Hotspot (up to step 4)</t>
+  </si>
+  <si>
+    <t>http://raspberrypihq.com/how-to-share-a-folder-with-a-windows-computer-from-a-raspberry-pi/</t>
+  </si>
+  <si>
+    <t>Setup samba share</t>
   </si>
 </sst>
 </file>
@@ -396,15 +402,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -441,14 +448,23 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Deleted Arduino scripts, corrected password
</commit_message>
<xml_diff>
--- a/Datalogger V2/Commands.xlsx
+++ b/Datalogger V2/Commands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>sudo apt-get update; sudo apt-get upgrade</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Setup samba share</t>
+  </si>
+  <si>
+    <t>Chmod 0777 on the folder that is being samba shared.</t>
+  </si>
+  <si>
+    <t>http://ubuntuforums.org/showthread.php?t=1723762</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +462,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>

</xml_diff>

<commit_message>
Testing realtime script in a vehicle
</commit_message>
<xml_diff>
--- a/Datalogger V2/Commands.xlsx
+++ b/Datalogger V2/Commands.xlsx
@@ -36,12 +36,6 @@
     <t>installed can functionality</t>
   </si>
   <si>
-    <t>http://elinux.org/RPI-Wireless-Hotspot</t>
-  </si>
-  <si>
-    <t>setup RPI-Wireless_Hotspot (up to step 4)</t>
-  </si>
-  <si>
     <t>http://raspberrypihq.com/how-to-share-a-folder-with-a-windows-computer-from-a-raspberry-pi/</t>
   </si>
   <si>
@@ -52,6 +46,12 @@
   </si>
   <si>
     <t>http://ubuntuforums.org/showthread.php?t=1723762</t>
+  </si>
+  <si>
+    <t>https://learn.adafruit.com/setting-up-a-raspberry-pi-as-a-wifi-access-point/install-software</t>
+  </si>
+  <si>
+    <t>setup hotspot</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,37 +448,36 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added support scripts (ensure logging, etc).
</commit_message>
<xml_diff>
--- a/Datalogger V2/Commands.xlsx
+++ b/Datalogger V2/Commands.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>sudo apt-get update; sudo apt-get upgrade</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>http://www.domoticz.com/wiki/Setting_up_a_RAM_drive_on_Raspberry_Pi</t>
+  </si>
+  <si>
+    <t>http://www.opentechguides.com/how-to/article/raspberry-pi/5/raspberry-pi-auto-start.html</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>https://learn.adafruit.com/adding-a-real-time-clock-to-raspberry-pi?view=all</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -414,74 +426,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -490,9 +587,12 @@
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B6" r:id="rId3"/>
     <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>